<commit_message>
[FIX] filter charge_type (expense, gl, revenue and trial balance web)
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_expense_ledger.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_expense_ledger.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t xml:space="preserve">Expense Ledger Report</t>
   </si>
@@ -55,13 +55,13 @@
     <t xml:space="preserve">Date To</t>
   </si>
   <si>
+    <t xml:space="preserve">Charge Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Run By</t>
   </si>
   <si>
     <t xml:space="preserve">Run Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge Type</t>
   </si>
   <si>
     <t xml:space="preserve">Account Name</t>
@@ -381,12 +381,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -396,7 +396,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX13"/>
+  <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -948,10 +948,10 @@
       <c r="AX9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
@@ -1005,7 +1005,7 @@
       <c r="A11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
@@ -1055,9 +1055,11 @@
       <c r="AW11" s="0"/>
       <c r="AX11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12"/>
       <c r="C12" s="0"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
@@ -1107,155 +1109,207 @@
       <c r="AW12" s="0"/>
       <c r="AX12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="14" t="s">
+    <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="Z13" s="0"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="0"/>
+      <c r="AC13" s="0"/>
+      <c r="AD13" s="0"/>
+      <c r="AE13" s="0"/>
+      <c r="AF13" s="0"/>
+      <c r="AG13" s="0"/>
+      <c r="AH13" s="0"/>
+      <c r="AI13" s="0"/>
+      <c r="AJ13" s="0"/>
+      <c r="AK13" s="0"/>
+      <c r="AL13" s="0"/>
+      <c r="AM13" s="0"/>
+      <c r="AN13" s="0"/>
+      <c r="AO13" s="0"/>
+      <c r="AP13" s="0"/>
+      <c r="AQ13" s="0"/>
+      <c r="AR13" s="0"/>
+      <c r="AS13" s="0"/>
+      <c r="AT13" s="0"/>
+      <c r="AU13" s="0"/>
+      <c r="AV13" s="0"/>
+      <c r="AW13" s="0"/>
+      <c r="AX13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="M14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="14" t="s">
+      <c r="N14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="O14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="Q13" s="14" t="s">
+      <c r="Q14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="R13" s="14" t="s">
+      <c r="R14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="S13" s="14" t="s">
+      <c r="S14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="T13" s="14" t="s">
+      <c r="T14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="U13" s="14" t="s">
+      <c r="U14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="V13" s="14" t="s">
+      <c r="V14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="W13" s="14" t="s">
+      <c r="W14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="X13" s="14" t="s">
+      <c r="X14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Y13" s="14" t="s">
+      <c r="Y14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="Z13" s="14" t="s">
+      <c r="Z14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AA13" s="14" t="s">
+      <c r="AA14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AB13" s="14" t="s">
+      <c r="AB14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AC13" s="14" t="s">
+      <c r="AC14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AD13" s="14" t="s">
+      <c r="AD14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AE13" s="14" t="s">
+      <c r="AE14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AF13" s="14" t="s">
+      <c r="AF14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AG13" s="14" t="s">
+      <c r="AG14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AH13" s="14" t="s">
+      <c r="AH14" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AI13" s="14" t="s">
+      <c r="AI14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AJ13" s="14" t="s">
+      <c r="AJ14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AK13" s="14" t="s">
+      <c r="AK14" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AL13" s="14" t="s">
+      <c r="AL14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AM13" s="14" t="s">
+      <c r="AM14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AN13" s="14" t="s">
+      <c r="AN14" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="AO13" s="14" t="s">
+      <c r="AO14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="AP13" s="14" t="s">
+      <c r="AP14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AQ13" s="14" t="s">
+      <c r="AQ14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AR13" s="14" t="s">
+      <c r="AR14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AS13" s="14" t="s">
+      <c r="AS14" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="AT13" s="14" t="s">
+      <c r="AT14" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AU13" s="14" t="s">
+      <c r="AU14" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AV13" s="14" t="s">
+      <c r="AV14" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="AW13" s="14" t="s">
+      <c r="AW14" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AX13" s="14" t="s">
+      <c r="AX14" s="14" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>